<commit_message>
Alteração a miu.xls (Apenas formatação, valores não intocados)
</commit_message>
<xml_diff>
--- a/spreadsheets/DistChegadas.xlsx
+++ b/spreadsheets/DistChegadas.xlsx
@@ -31,7 +31,27 @@
     <t>Soma(t)</t>
   </si>
   <si>
-    <t>Taxa de chegada (Lambda)</t>
+    <r>
+      <t xml:space="preserve">Taxa de chegada (</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Ubuntu"/>
+        <charset val="1"/>
+        <family val="0"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve">λ</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <sz val="10"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t>Número de Categorias</t>
@@ -58,7 +78,7 @@
     <t>L4</t>
   </si>
   <si>
-    <t>Categoria </t>
+    <t>Categoria</t>
   </si>
   <si>
     <t>Número observado</t>
@@ -107,7 +127,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -126,6 +146,12 @@
     </font>
     <font>
       <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Ubuntu"/>
+      <charset val="1"/>
       <family val="0"/>
       <sz val="10"/>
     </font>
@@ -216,8 +242,8 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="4" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -302,17 +328,17 @@
   </sheetPr>
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A13" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C38" activeCellId="0" pane="topLeft" sqref="C38:I38"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G10" activeCellId="0" pane="topLeft" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.0823529411765"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.6941176470588"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3529411764706"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1921568627451"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -5519,11 +5545,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C38:I38 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5544,11 +5570,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="C38:I38 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Alterações a DistChegadas.xlsx e miu.xlsx
</commit_message>
<xml_diff>
--- a/spreadsheets/DistChegadas.xlsx
+++ b/spreadsheets/DistChegadas.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>MEIO-TP1</t>
   </si>
@@ -28,11 +28,11 @@
     <t>Número de observações</t>
   </si>
   <si>
-    <t>Soma(t)</t>
+    <t>Soma dos intervalos de tempo entre chegadas (segundos)</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Taxa de chegada (</t>
+      <t xml:space="preserve">Taxa de chegada </t>
     </r>
     <r>
       <rPr>
@@ -41,16 +41,21 @@
         <family val="0"/>
         <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">λ</t>
+      <t xml:space="preserve">λ (chegada/segundo)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Taxa de chegada </t>
     </r>
     <r>
       <rPr>
-        <rFont val="Arial"/>
+        <rFont val="Ubuntu"/>
         <charset val="1"/>
-        <family val="2"/>
+        <family val="0"/>
         <sz val="10"/>
       </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve">λ (chegada/hora)</t>
     </r>
   </si>
   <si>
@@ -127,7 +132,7 @@
   <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
       <charset val="1"/>
@@ -153,6 +158,11 @@
       <name val="Ubuntu"/>
       <charset val="1"/>
       <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
       <sz val="10"/>
     </font>
     <font>
@@ -224,7 +234,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="2" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
@@ -242,8 +252,11 @@
     <xf applyAlignment="true" applyBorder="true" applyFont="false" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="5" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="3" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="center" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="1" fillId="0" fontId="0" numFmtId="164" xfId="0">
@@ -328,17 +341,17 @@
   </sheetPr>
   <dimension ref="A1:I1002"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G10" activeCellId="0" pane="topLeft" sqref="G10"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A10" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="E25" activeCellId="0" pane="topLeft" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.1921568627451"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.4352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="50.4039215686275"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.2980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.5137254901961"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -412,6 +425,13 @@
       <c r="A8" s="3" t="n">
         <v>0.2</v>
       </c>
+      <c r="C8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <f aca="false">D7*60*60</f>
+        <v>208.641224028514</v>
+      </c>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
@@ -426,12 +446,6 @@
       <c r="A10" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
@@ -439,12 +453,11 @@
       <c r="A11" s="3" t="n">
         <v>0.3</v>
       </c>
-      <c r="C11" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="D11" s="6" t="n">
-        <f aca="false">PRODUCT((1/C11), D5)</f>
-        <v>200</v>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -453,6 +466,13 @@
       <c r="A12" s="3" t="n">
         <v>0.3</v>
       </c>
+      <c r="C12" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <f aca="false">PRODUCT((1/C12), D5)</f>
+        <v>200</v>
+      </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
@@ -460,29 +480,22 @@
       <c r="A13" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
       <c r="A14" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
       <c r="A15" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D15" s="6" t="n">
-        <v>3.847</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
@@ -492,8 +505,9 @@
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="6" t="n">
-        <v>8.807</v>
+      <c r="D16" s="7" t="n">
+        <f aca="false">LN(0.8 )/(-D7)</f>
+        <v>3.85023040615103</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
@@ -504,7 +518,8 @@
         <v>11</v>
       </c>
       <c r="D17" s="6" t="n">
-        <v>15.798</v>
+        <f aca="false">LN(0.6 )/(-D7)</f>
+        <v>8.81404072527029</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
@@ -515,13 +530,21 @@
         <v>12</v>
       </c>
       <c r="D18" s="6" t="n">
-        <v>27.749</v>
+        <f aca="false">LN(0.4 )/(-D7)</f>
+        <v>15.8101384331226</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="3" t="n">
         <v>0.5</v>
       </c>
+      <c r="C19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="6" t="n">
+        <f aca="false">LN(0.2 )/(-D7)</f>
+        <v>27.7700464600942</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="3" t="n">
@@ -532,22 +555,16 @@
       <c r="A21" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="3" t="n">
         <v>0.6</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D22" s="6" t="n">
-        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="23">
@@ -558,7 +575,7 @@
         <v>16</v>
       </c>
       <c r="D23" s="6" t="n">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="24">
@@ -569,7 +586,7 @@
         <v>17</v>
       </c>
       <c r="D24" s="6" t="n">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="25">
@@ -580,7 +597,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="6" t="n">
-        <v>224</v>
+        <v>215</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="26">
@@ -591,14 +608,20 @@
         <v>19</v>
       </c>
       <c r="D26" s="6" t="n">
-        <v>185</v>
-      </c>
-      <c r="I26" s="7"/>
+        <v>221</v>
+      </c>
+      <c r="I26" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="27">
       <c r="A27" s="3" t="n">
         <v>0.7</v>
       </c>
+      <c r="C27" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="6" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="28">
       <c r="A28" s="3" t="n">
@@ -609,10 +632,6 @@
       <c r="A29" s="3" t="n">
         <v>0.8</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="8"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="30">
       <c r="A30" s="3" t="n">
@@ -621,74 +640,78 @@
       <c r="C30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="9" t="n">
-        <f aca="false">POWER((D22-D11),2)/D11</f>
-        <v>0.845</v>
-      </c>
+      <c r="D30" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="31">
       <c r="A31" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="9" t="n">
-        <f aca="false">POWER((D23-D11),2)/D11</f>
-        <v>0.32</v>
+      <c r="D31" s="10" t="n">
+        <f aca="false">POWER((D23-D12),2)/D12</f>
+        <v>0.845</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="32">
       <c r="A32" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C32" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D32" s="9" t="n">
-        <f aca="false">POWER((D24-D11),2)/D11</f>
-        <v>0.72</v>
+      <c r="D32" s="10" t="n">
+        <f aca="false">POWER((D24-D12),2)/D12</f>
+        <v>0.32</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
       <c r="A33" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C33" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="9" t="n">
-        <f aca="false">POWER((D25-D11),2)/D11</f>
-        <v>2.88</v>
+      <c r="D33" s="10" t="n">
+        <f aca="false">POWER((D25-D12),2)/D12</f>
+        <v>1.125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="34">
       <c r="A34" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="9" t="n">
-        <f aca="false">POWER((D26-D11),2)/D11</f>
-        <v>1.125</v>
+      <c r="D34" s="10" t="n">
+        <f aca="false">POWER((D26-D12),2)/D12</f>
+        <v>2.205</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="35">
       <c r="A35" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="9" t="n">
-        <f aca="false">SUM(D30:D34)</f>
-        <v>5.89</v>
+      <c r="D35" s="10" t="n">
+        <f aca="false">POWER((D27-D12),2)/D12</f>
+        <v>1.125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="36">
       <c r="A36" s="3" t="n">
         <v>0.9</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="10" t="n">
+        <f aca="false">SUM(D31:D35)</f>
+        <v>5.62</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="37">
@@ -5525,7 +5548,7 @@
   <mergeCells count="3">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -5549,7 +5572,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5574,7 +5597,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>